<commit_message>
Updating taxonomies and rqs
</commit_message>
<xml_diff>
--- a/7_Data_Extraction/Data_Extraction_Antonio.xlsx
+++ b/7_Data_Extraction/Data_Extraction_Antonio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antoniotrovato/Documents/GitHub/RegressionTestingOptimizationSLR/7_Data_Extraction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF866389-C561-A344-989E-F9A6DCB4B595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41748892-67E4-6840-ACCF-49487A14C08A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="464">
   <si>
     <t>ID</t>
   </si>
@@ -1415,13 +1415,16 @@
     <t>RQ2.2</t>
   </si>
   <si>
-    <t>RQ4.1</t>
-  </si>
-  <si>
-    <t>RQ4.2</t>
-  </si>
-  <si>
-    <t>RQ3</t>
+    <t>RQ1.3a</t>
+  </si>
+  <si>
+    <t>RQ2.3</t>
+  </si>
+  <si>
+    <t>RQ3.1</t>
+  </si>
+  <si>
+    <t>RQ3.2</t>
   </si>
 </sst>
 </file>
@@ -1795,15 +1798,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AV52"/>
+  <dimension ref="A1:AW52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
-      <selection activeCell="AO1" sqref="AO1:AV1048576"/>
+      <selection activeCell="AG8" sqref="AG8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1934,22 +1937,25 @@
         <v>457</v>
       </c>
       <c r="AR1" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="AS1" s="1" t="s">
         <v>458</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="AV1" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="AU1" s="1" t="s">
-        <v>460</v>
-      </c>
-      <c r="AV1" s="1" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AW1" s="1" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="2" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>9068003</v>
       </c>
@@ -1990,7 +1996,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>9022761</v>
       </c>
@@ -2034,7 +2040,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>7561371</v>
       </c>
@@ -2075,7 +2081,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>6884931</v>
       </c>
@@ -2116,7 +2122,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>10048797</v>
       </c>
@@ -2157,7 +2163,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>8377903</v>
       </c>
@@ -2204,7 +2210,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7045344</v>
       </c>
@@ -2245,7 +2251,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>9198020</v>
       </c>
@@ -2286,7 +2292,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="10" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8776936</v>
       </c>
@@ -2327,7 +2333,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="11" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10197719</v>
       </c>
@@ -2371,7 +2377,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="12" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>8261011</v>
       </c>
@@ -2412,7 +2418,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="13" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>9160217</v>
       </c>
@@ -2453,7 +2459,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="14" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>8229925</v>
       </c>
@@ -2494,7 +2500,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="15" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>7207103</v>
       </c>
@@ -2535,7 +2541,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="16" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>7515934</v>
       </c>

</xml_diff>